<commit_message>
Removed B and V from HMXBparameters.xlsx and added references to the data. Also added Porbit and Pspin to falenga
</commit_message>
<xml_diff>
--- a/tables/M_expBONNSAI.xlsx
+++ b/tables/M_expBONNSAI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15D58D7-E7F5-40ED-8A61-81FBC803E2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFE9F68-EC50-474F-B47A-4CFDA58B601B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{263918F3-A67B-4C3D-8EE7-D7BA132604BB}"/>
+    <workbookView xWindow="7200" yWindow="4035" windowWidth="21600" windowHeight="11265" xr2:uid="{263918F3-A67B-4C3D-8EE7-D7BA132604BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>id</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>OAO 1657-415</t>
+  </si>
+  <si>
+    <t>M_HRD</t>
   </si>
 </sst>
 </file>
@@ -424,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538169ED-C2F3-40D5-88B5-FFFF0369ADB9}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -435,79 +438,107 @@
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>28.8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>38.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>21.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>35.799999999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>22.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>126.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>39</v>
+      </c>
+      <c r="C7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>21.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9">
         <v>8.8000000000000007</v>
       </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added a function that handles asymmetric errors, but this has still to be implemented in luminosity.ipynb
</commit_message>
<xml_diff>
--- a/tables/M_expBONNSAI.xlsx
+++ b/tables/M_expBONNSAI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFE9F68-EC50-474F-B47A-4CFDA58B601B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DF1143-5FA6-494C-A3DC-82264B42850D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4035" windowWidth="21600" windowHeight="11265" xr2:uid="{263918F3-A67B-4C3D-8EE7-D7BA132604BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{263918F3-A67B-4C3D-8EE7-D7BA132604BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>id</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>M_HRD</t>
+  </si>
+  <si>
+    <t>M_exp_err</t>
   </si>
 </sst>
 </file>
@@ -427,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538169ED-C2F3-40D5-88B5-FFFF0369ADB9}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -438,7 +441,7 @@
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,85 +451,109 @@
       <c r="C1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>28.8</v>
+        <v>31.2</v>
       </c>
       <c r="C2">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>38.4</v>
+        <v>35.4</v>
       </c>
       <c r="C3">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>21.8</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="C4">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>35.799999999999997</v>
+        <v>44</v>
       </c>
       <c r="C5">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>22.4</v>
+        <v>19.8</v>
       </c>
       <c r="C6">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>39</v>
+        <v>46.4</v>
       </c>
       <c r="C7">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>21.2</v>
+        <v>21.6</v>
       </c>
       <c r="C8">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -535,6 +562,9 @@
       </c>
       <c r="C9">
         <v>12</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>